<commit_message>
Included dynamic colors for gant
</commit_message>
<xml_diff>
--- a/data/InputData.xlsx
+++ b/data/InputData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Denis\python\workforce_scheduling\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-20.04\home\renzo\PycharmProjects\workforce_scheduling\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06817145-2D20-4DA3-8E49-22CB4F1B07B6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39475F36-6460-4279-BCAF-FD47D73E0BC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-119" yWindow="-119" windowWidth="25603" windowHeight="13898" xr2:uid="{BCDF856C-6F0D-487F-8BC7-04FD1FA73F2E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="4" xr2:uid="{BCDF856C-6F0D-487F-8BC7-04FD1FA73F2E}"/>
   </bookViews>
   <sheets>
     <sheet name="Employees" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="88">
   <si>
     <t>Name</t>
   </si>
@@ -134,6 +134,171 @@
   </si>
   <si>
     <t>Ruth</t>
+  </si>
+  <si>
+    <t>Sunday</t>
+  </si>
+  <si>
+    <t>Mark</t>
+  </si>
+  <si>
+    <t>Helen</t>
+  </si>
+  <si>
+    <t>James</t>
+  </si>
+  <si>
+    <t>Susan</t>
+  </si>
+  <si>
+    <t>Robert</t>
+  </si>
+  <si>
+    <t>Anna</t>
+  </si>
+  <si>
+    <t>David</t>
+  </si>
+  <si>
+    <t>Laura</t>
+  </si>
+  <si>
+    <t>Michael</t>
+  </si>
+  <si>
+    <t>Grace</t>
+  </si>
+  <si>
+    <t>Charles</t>
+  </si>
+  <si>
+    <t>Emma</t>
+  </si>
+  <si>
+    <t>Peter</t>
+  </si>
+  <si>
+    <t>Nancy</t>
+  </si>
+  <si>
+    <t>Thomas</t>
+  </si>
+  <si>
+    <t>Julie</t>
+  </si>
+  <si>
+    <t>Daniel</t>
+  </si>
+  <si>
+    <t>Sarah</t>
+  </si>
+  <si>
+    <t>Andrew</t>
+  </si>
+  <si>
+    <t>Clara</t>
+  </si>
+  <si>
+    <t>Brian</t>
+  </si>
+  <si>
+    <t>Olivia</t>
+  </si>
+  <si>
+    <t>George</t>
+  </si>
+  <si>
+    <t>Alice</t>
+  </si>
+  <si>
+    <t>Kevin</t>
+  </si>
+  <si>
+    <t>Diana</t>
+  </si>
+  <si>
+    <t>Edward</t>
+  </si>
+  <si>
+    <t>Rachel</t>
+  </si>
+  <si>
+    <t>Henry</t>
+  </si>
+  <si>
+    <t>Sophie</t>
+  </si>
+  <si>
+    <t>Jason</t>
+  </si>
+  <si>
+    <t>Victoria</t>
+  </si>
+  <si>
+    <t>Samuel</t>
+  </si>
+  <si>
+    <t>Eva</t>
+  </si>
+  <si>
+    <t>Matthew</t>
+  </si>
+  <si>
+    <t>Nora</t>
+  </si>
+  <si>
+    <t>Anthony</t>
+  </si>
+  <si>
+    <t>Megan</t>
+  </si>
+  <si>
+    <t>Christopher</t>
+  </si>
+  <si>
+    <t>Irene</t>
+  </si>
+  <si>
+    <t>Joseph</t>
+  </si>
+  <si>
+    <t>Amy</t>
+  </si>
+  <si>
+    <t>Benjamin</t>
+  </si>
+  <si>
+    <t>Ella</t>
+  </si>
+  <si>
+    <t>Patrick</t>
+  </si>
+  <si>
+    <t>Isabel</t>
+  </si>
+  <si>
+    <t>Nathan</t>
+  </si>
+  <si>
+    <t>Lucy</t>
+  </si>
+  <si>
+    <t>Philip</t>
+  </si>
+  <si>
+    <t>Tina</t>
+  </si>
+  <si>
+    <t>Simon</t>
+  </si>
+  <si>
+    <t>Nicole</t>
+  </si>
+  <si>
+    <t>Jacob</t>
+  </si>
+  <si>
+    <t>Leah</t>
   </si>
 </sst>
 </file>
@@ -199,7 +364,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -208,10 +373,9 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -227,9 +391,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -267,7 +431,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -373,7 +537,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -515,7 +679,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -523,21 +687,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56438F95-CB28-49F8-8745-B51411212C3C}">
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:K63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2:K63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.2" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.5546875" customWidth="1"/>
-    <col min="2" max="2" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.33203125" customWidth="1"/>
-    <col min="10" max="10" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.5703125" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.28515625" customWidth="1"/>
+    <col min="11" max="11" width="17.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -562,14 +726,17 @@
       <c r="H1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="J1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="J1" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K1" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>26</v>
       </c>
@@ -577,7 +744,7 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D2">
         <v>8</v>
@@ -595,13 +762,16 @@
         <v>8</v>
       </c>
       <c r="I2">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="J2">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+      <c r="K2">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -609,10 +779,10 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E3">
         <v>8</v>
@@ -627,13 +797,16 @@
         <v>8</v>
       </c>
       <c r="I3">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="J3">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+      <c r="K3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>28</v>
       </c>
@@ -659,13 +832,16 @@
         <v>8</v>
       </c>
       <c r="I4">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="J4">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+      <c r="K4">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>29</v>
       </c>
@@ -691,13 +867,16 @@
         <v>8</v>
       </c>
       <c r="I5">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="J5">
-        <v>37.5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+      <c r="K5">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -714,7 +893,7 @@
         <v>8</v>
       </c>
       <c r="F6">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="G6">
         <v>8</v>
@@ -723,13 +902,16 @@
         <v>8</v>
       </c>
       <c r="I6">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="J6">
-        <v>37.5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+      <c r="K6">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>30</v>
       </c>
@@ -737,31 +919,34 @@
         <v>0</v>
       </c>
       <c r="C7">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D7">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E7">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F7">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="G7">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="H7">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="I7">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="J7">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+      <c r="K7">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>31</v>
       </c>
@@ -769,31 +954,34 @@
         <v>1</v>
       </c>
       <c r="C8">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D8">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E8">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F8">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="G8">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="H8">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="I8">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="J8">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+      <c r="K8">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>32</v>
       </c>
@@ -801,28 +989,1921 @@
         <v>0</v>
       </c>
       <c r="C9">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D9">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E9">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F9">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="G9">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="H9">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="I9">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="J9">
-        <v>20</v>
+        <v>44</v>
+      </c>
+      <c r="K9">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>8</v>
+      </c>
+      <c r="D10">
+        <v>8</v>
+      </c>
+      <c r="E10">
+        <v>8</v>
+      </c>
+      <c r="F10">
+        <v>8</v>
+      </c>
+      <c r="G10">
+        <v>8</v>
+      </c>
+      <c r="H10">
+        <v>8</v>
+      </c>
+      <c r="I10">
+        <v>8</v>
+      </c>
+      <c r="J10">
+        <v>44</v>
+      </c>
+      <c r="K10">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>8</v>
+      </c>
+      <c r="D11">
+        <v>8</v>
+      </c>
+      <c r="E11">
+        <v>8</v>
+      </c>
+      <c r="F11">
+        <v>8</v>
+      </c>
+      <c r="G11">
+        <v>8</v>
+      </c>
+      <c r="H11">
+        <v>8</v>
+      </c>
+      <c r="I11">
+        <v>8</v>
+      </c>
+      <c r="J11">
+        <v>44</v>
+      </c>
+      <c r="K11">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>8</v>
+      </c>
+      <c r="D12">
+        <v>8</v>
+      </c>
+      <c r="E12">
+        <v>8</v>
+      </c>
+      <c r="F12">
+        <v>8</v>
+      </c>
+      <c r="G12">
+        <v>8</v>
+      </c>
+      <c r="H12">
+        <v>8</v>
+      </c>
+      <c r="I12">
+        <v>8</v>
+      </c>
+      <c r="J12">
+        <v>44</v>
+      </c>
+      <c r="K12">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>8</v>
+      </c>
+      <c r="D13">
+        <v>8</v>
+      </c>
+      <c r="E13">
+        <v>8</v>
+      </c>
+      <c r="F13">
+        <v>8</v>
+      </c>
+      <c r="G13">
+        <v>8</v>
+      </c>
+      <c r="H13">
+        <v>8</v>
+      </c>
+      <c r="I13">
+        <v>8</v>
+      </c>
+      <c r="J13">
+        <v>44</v>
+      </c>
+      <c r="K13">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>8</v>
+      </c>
+      <c r="D14">
+        <v>8</v>
+      </c>
+      <c r="E14">
+        <v>8</v>
+      </c>
+      <c r="F14">
+        <v>8</v>
+      </c>
+      <c r="G14">
+        <v>8</v>
+      </c>
+      <c r="H14">
+        <v>8</v>
+      </c>
+      <c r="I14">
+        <v>8</v>
+      </c>
+      <c r="J14">
+        <v>44</v>
+      </c>
+      <c r="K14">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>8</v>
+      </c>
+      <c r="D15">
+        <v>8</v>
+      </c>
+      <c r="E15">
+        <v>8</v>
+      </c>
+      <c r="F15">
+        <v>8</v>
+      </c>
+      <c r="G15">
+        <v>8</v>
+      </c>
+      <c r="H15">
+        <v>8</v>
+      </c>
+      <c r="I15">
+        <v>8</v>
+      </c>
+      <c r="J15">
+        <v>44</v>
+      </c>
+      <c r="K15">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>8</v>
+      </c>
+      <c r="D16">
+        <v>8</v>
+      </c>
+      <c r="E16">
+        <v>8</v>
+      </c>
+      <c r="F16">
+        <v>8</v>
+      </c>
+      <c r="G16">
+        <v>8</v>
+      </c>
+      <c r="H16">
+        <v>8</v>
+      </c>
+      <c r="I16">
+        <v>8</v>
+      </c>
+      <c r="J16">
+        <v>44</v>
+      </c>
+      <c r="K16">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>8</v>
+      </c>
+      <c r="D17">
+        <v>8</v>
+      </c>
+      <c r="E17">
+        <v>8</v>
+      </c>
+      <c r="F17">
+        <v>8</v>
+      </c>
+      <c r="G17">
+        <v>8</v>
+      </c>
+      <c r="H17">
+        <v>8</v>
+      </c>
+      <c r="I17">
+        <v>8</v>
+      </c>
+      <c r="J17">
+        <v>44</v>
+      </c>
+      <c r="K17">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>42</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>8</v>
+      </c>
+      <c r="D18">
+        <v>8</v>
+      </c>
+      <c r="E18">
+        <v>8</v>
+      </c>
+      <c r="F18">
+        <v>8</v>
+      </c>
+      <c r="G18">
+        <v>8</v>
+      </c>
+      <c r="H18">
+        <v>8</v>
+      </c>
+      <c r="I18">
+        <v>8</v>
+      </c>
+      <c r="J18">
+        <v>44</v>
+      </c>
+      <c r="K18">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <v>8</v>
+      </c>
+      <c r="D19">
+        <v>8</v>
+      </c>
+      <c r="E19">
+        <v>8</v>
+      </c>
+      <c r="F19">
+        <v>8</v>
+      </c>
+      <c r="G19">
+        <v>8</v>
+      </c>
+      <c r="H19">
+        <v>8</v>
+      </c>
+      <c r="I19">
+        <v>8</v>
+      </c>
+      <c r="J19">
+        <v>44</v>
+      </c>
+      <c r="K19">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>44</v>
+      </c>
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <v>8</v>
+      </c>
+      <c r="D20">
+        <v>8</v>
+      </c>
+      <c r="E20">
+        <v>8</v>
+      </c>
+      <c r="F20">
+        <v>8</v>
+      </c>
+      <c r="G20">
+        <v>8</v>
+      </c>
+      <c r="H20">
+        <v>8</v>
+      </c>
+      <c r="I20">
+        <v>8</v>
+      </c>
+      <c r="J20">
+        <v>44</v>
+      </c>
+      <c r="K20">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>45</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+      <c r="C21">
+        <v>8</v>
+      </c>
+      <c r="D21">
+        <v>8</v>
+      </c>
+      <c r="E21">
+        <v>8</v>
+      </c>
+      <c r="F21">
+        <v>8</v>
+      </c>
+      <c r="G21">
+        <v>8</v>
+      </c>
+      <c r="H21">
+        <v>8</v>
+      </c>
+      <c r="I21">
+        <v>8</v>
+      </c>
+      <c r="J21">
+        <v>44</v>
+      </c>
+      <c r="K21">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>46</v>
+      </c>
+      <c r="B22">
+        <v>0</v>
+      </c>
+      <c r="C22">
+        <v>8</v>
+      </c>
+      <c r="D22">
+        <v>8</v>
+      </c>
+      <c r="E22">
+        <v>8</v>
+      </c>
+      <c r="F22">
+        <v>8</v>
+      </c>
+      <c r="G22">
+        <v>8</v>
+      </c>
+      <c r="H22">
+        <v>8</v>
+      </c>
+      <c r="I22">
+        <v>8</v>
+      </c>
+      <c r="J22">
+        <v>44</v>
+      </c>
+      <c r="K22">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>47</v>
+      </c>
+      <c r="B23">
+        <v>0</v>
+      </c>
+      <c r="C23">
+        <v>8</v>
+      </c>
+      <c r="D23">
+        <v>8</v>
+      </c>
+      <c r="E23">
+        <v>8</v>
+      </c>
+      <c r="F23">
+        <v>8</v>
+      </c>
+      <c r="G23">
+        <v>8</v>
+      </c>
+      <c r="H23">
+        <v>8</v>
+      </c>
+      <c r="I23">
+        <v>8</v>
+      </c>
+      <c r="J23">
+        <v>44</v>
+      </c>
+      <c r="K23">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>48</v>
+      </c>
+      <c r="B24">
+        <v>0</v>
+      </c>
+      <c r="C24">
+        <v>8</v>
+      </c>
+      <c r="D24">
+        <v>8</v>
+      </c>
+      <c r="E24">
+        <v>8</v>
+      </c>
+      <c r="F24">
+        <v>8</v>
+      </c>
+      <c r="G24">
+        <v>8</v>
+      </c>
+      <c r="H24">
+        <v>8</v>
+      </c>
+      <c r="I24">
+        <v>8</v>
+      </c>
+      <c r="J24">
+        <v>44</v>
+      </c>
+      <c r="K24">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>49</v>
+      </c>
+      <c r="B25">
+        <v>0</v>
+      </c>
+      <c r="C25">
+        <v>8</v>
+      </c>
+      <c r="D25">
+        <v>8</v>
+      </c>
+      <c r="E25">
+        <v>8</v>
+      </c>
+      <c r="F25">
+        <v>8</v>
+      </c>
+      <c r="G25">
+        <v>8</v>
+      </c>
+      <c r="H25">
+        <v>8</v>
+      </c>
+      <c r="I25">
+        <v>8</v>
+      </c>
+      <c r="J25">
+        <v>44</v>
+      </c>
+      <c r="K25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>50</v>
+      </c>
+      <c r="B26">
+        <v>0</v>
+      </c>
+      <c r="C26">
+        <v>8</v>
+      </c>
+      <c r="D26">
+        <v>8</v>
+      </c>
+      <c r="E26">
+        <v>8</v>
+      </c>
+      <c r="F26">
+        <v>8</v>
+      </c>
+      <c r="G26">
+        <v>8</v>
+      </c>
+      <c r="H26">
+        <v>8</v>
+      </c>
+      <c r="I26">
+        <v>8</v>
+      </c>
+      <c r="J26">
+        <v>44</v>
+      </c>
+      <c r="K26">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>51</v>
+      </c>
+      <c r="B27">
+        <v>0</v>
+      </c>
+      <c r="C27">
+        <v>8</v>
+      </c>
+      <c r="D27">
+        <v>8</v>
+      </c>
+      <c r="E27">
+        <v>8</v>
+      </c>
+      <c r="F27">
+        <v>8</v>
+      </c>
+      <c r="G27">
+        <v>8</v>
+      </c>
+      <c r="H27">
+        <v>8</v>
+      </c>
+      <c r="I27">
+        <v>8</v>
+      </c>
+      <c r="J27">
+        <v>44</v>
+      </c>
+      <c r="K27">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>52</v>
+      </c>
+      <c r="B28">
+        <v>0</v>
+      </c>
+      <c r="C28">
+        <v>8</v>
+      </c>
+      <c r="D28">
+        <v>8</v>
+      </c>
+      <c r="E28">
+        <v>8</v>
+      </c>
+      <c r="F28">
+        <v>8</v>
+      </c>
+      <c r="G28">
+        <v>8</v>
+      </c>
+      <c r="H28">
+        <v>8</v>
+      </c>
+      <c r="I28">
+        <v>8</v>
+      </c>
+      <c r="J28">
+        <v>44</v>
+      </c>
+      <c r="K28">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>53</v>
+      </c>
+      <c r="B29">
+        <v>0</v>
+      </c>
+      <c r="C29">
+        <v>8</v>
+      </c>
+      <c r="D29">
+        <v>8</v>
+      </c>
+      <c r="E29">
+        <v>8</v>
+      </c>
+      <c r="F29">
+        <v>8</v>
+      </c>
+      <c r="G29">
+        <v>8</v>
+      </c>
+      <c r="H29">
+        <v>8</v>
+      </c>
+      <c r="I29">
+        <v>8</v>
+      </c>
+      <c r="J29">
+        <v>44</v>
+      </c>
+      <c r="K29">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>54</v>
+      </c>
+      <c r="B30">
+        <v>0</v>
+      </c>
+      <c r="C30">
+        <v>8</v>
+      </c>
+      <c r="D30">
+        <v>8</v>
+      </c>
+      <c r="E30">
+        <v>8</v>
+      </c>
+      <c r="F30">
+        <v>8</v>
+      </c>
+      <c r="G30">
+        <v>8</v>
+      </c>
+      <c r="H30">
+        <v>8</v>
+      </c>
+      <c r="I30">
+        <v>8</v>
+      </c>
+      <c r="J30">
+        <v>44</v>
+      </c>
+      <c r="K30">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>55</v>
+      </c>
+      <c r="B31">
+        <v>0</v>
+      </c>
+      <c r="C31">
+        <v>8</v>
+      </c>
+      <c r="D31">
+        <v>8</v>
+      </c>
+      <c r="E31">
+        <v>8</v>
+      </c>
+      <c r="F31">
+        <v>8</v>
+      </c>
+      <c r="G31">
+        <v>8</v>
+      </c>
+      <c r="H31">
+        <v>8</v>
+      </c>
+      <c r="I31">
+        <v>8</v>
+      </c>
+      <c r="J31">
+        <v>44</v>
+      </c>
+      <c r="K31">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>56</v>
+      </c>
+      <c r="B32">
+        <v>0</v>
+      </c>
+      <c r="C32">
+        <v>8</v>
+      </c>
+      <c r="D32">
+        <v>8</v>
+      </c>
+      <c r="E32">
+        <v>8</v>
+      </c>
+      <c r="F32">
+        <v>8</v>
+      </c>
+      <c r="G32">
+        <v>8</v>
+      </c>
+      <c r="H32">
+        <v>8</v>
+      </c>
+      <c r="I32">
+        <v>8</v>
+      </c>
+      <c r="J32">
+        <v>44</v>
+      </c>
+      <c r="K32">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>57</v>
+      </c>
+      <c r="B33">
+        <v>0</v>
+      </c>
+      <c r="C33">
+        <v>8</v>
+      </c>
+      <c r="D33">
+        <v>8</v>
+      </c>
+      <c r="E33">
+        <v>8</v>
+      </c>
+      <c r="F33">
+        <v>8</v>
+      </c>
+      <c r="G33">
+        <v>8</v>
+      </c>
+      <c r="H33">
+        <v>8</v>
+      </c>
+      <c r="I33">
+        <v>8</v>
+      </c>
+      <c r="J33">
+        <v>44</v>
+      </c>
+      <c r="K33">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>58</v>
+      </c>
+      <c r="B34">
+        <v>0</v>
+      </c>
+      <c r="C34">
+        <v>8</v>
+      </c>
+      <c r="D34">
+        <v>8</v>
+      </c>
+      <c r="E34">
+        <v>8</v>
+      </c>
+      <c r="F34">
+        <v>8</v>
+      </c>
+      <c r="G34">
+        <v>8</v>
+      </c>
+      <c r="H34">
+        <v>8</v>
+      </c>
+      <c r="I34">
+        <v>8</v>
+      </c>
+      <c r="J34">
+        <v>44</v>
+      </c>
+      <c r="K34">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>59</v>
+      </c>
+      <c r="B35">
+        <v>0</v>
+      </c>
+      <c r="C35">
+        <v>8</v>
+      </c>
+      <c r="D35">
+        <v>8</v>
+      </c>
+      <c r="E35">
+        <v>8</v>
+      </c>
+      <c r="F35">
+        <v>8</v>
+      </c>
+      <c r="G35">
+        <v>8</v>
+      </c>
+      <c r="H35">
+        <v>8</v>
+      </c>
+      <c r="I35">
+        <v>8</v>
+      </c>
+      <c r="J35">
+        <v>44</v>
+      </c>
+      <c r="K35">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>60</v>
+      </c>
+      <c r="B36">
+        <v>0</v>
+      </c>
+      <c r="C36">
+        <v>8</v>
+      </c>
+      <c r="D36">
+        <v>8</v>
+      </c>
+      <c r="E36">
+        <v>8</v>
+      </c>
+      <c r="F36">
+        <v>8</v>
+      </c>
+      <c r="G36">
+        <v>8</v>
+      </c>
+      <c r="H36">
+        <v>8</v>
+      </c>
+      <c r="I36">
+        <v>8</v>
+      </c>
+      <c r="J36">
+        <v>44</v>
+      </c>
+      <c r="K36">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>61</v>
+      </c>
+      <c r="B37">
+        <v>0</v>
+      </c>
+      <c r="C37">
+        <v>8</v>
+      </c>
+      <c r="D37">
+        <v>8</v>
+      </c>
+      <c r="E37">
+        <v>8</v>
+      </c>
+      <c r="F37">
+        <v>8</v>
+      </c>
+      <c r="G37">
+        <v>8</v>
+      </c>
+      <c r="H37">
+        <v>8</v>
+      </c>
+      <c r="I37">
+        <v>8</v>
+      </c>
+      <c r="J37">
+        <v>44</v>
+      </c>
+      <c r="K37">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>62</v>
+      </c>
+      <c r="B38">
+        <v>0</v>
+      </c>
+      <c r="C38">
+        <v>8</v>
+      </c>
+      <c r="D38">
+        <v>8</v>
+      </c>
+      <c r="E38">
+        <v>8</v>
+      </c>
+      <c r="F38">
+        <v>8</v>
+      </c>
+      <c r="G38">
+        <v>8</v>
+      </c>
+      <c r="H38">
+        <v>8</v>
+      </c>
+      <c r="I38">
+        <v>8</v>
+      </c>
+      <c r="J38">
+        <v>44</v>
+      </c>
+      <c r="K38">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>63</v>
+      </c>
+      <c r="B39">
+        <v>0</v>
+      </c>
+      <c r="C39">
+        <v>8</v>
+      </c>
+      <c r="D39">
+        <v>8</v>
+      </c>
+      <c r="E39">
+        <v>8</v>
+      </c>
+      <c r="F39">
+        <v>8</v>
+      </c>
+      <c r="G39">
+        <v>8</v>
+      </c>
+      <c r="H39">
+        <v>8</v>
+      </c>
+      <c r="I39">
+        <v>8</v>
+      </c>
+      <c r="J39">
+        <v>44</v>
+      </c>
+      <c r="K39">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>64</v>
+      </c>
+      <c r="B40">
+        <v>0</v>
+      </c>
+      <c r="C40">
+        <v>8</v>
+      </c>
+      <c r="D40">
+        <v>8</v>
+      </c>
+      <c r="E40">
+        <v>8</v>
+      </c>
+      <c r="F40">
+        <v>8</v>
+      </c>
+      <c r="G40">
+        <v>8</v>
+      </c>
+      <c r="H40">
+        <v>8</v>
+      </c>
+      <c r="I40">
+        <v>8</v>
+      </c>
+      <c r="J40">
+        <v>44</v>
+      </c>
+      <c r="K40">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>65</v>
+      </c>
+      <c r="B41">
+        <v>0</v>
+      </c>
+      <c r="C41">
+        <v>8</v>
+      </c>
+      <c r="D41">
+        <v>8</v>
+      </c>
+      <c r="E41">
+        <v>8</v>
+      </c>
+      <c r="F41">
+        <v>8</v>
+      </c>
+      <c r="G41">
+        <v>8</v>
+      </c>
+      <c r="H41">
+        <v>8</v>
+      </c>
+      <c r="I41">
+        <v>8</v>
+      </c>
+      <c r="J41">
+        <v>44</v>
+      </c>
+      <c r="K41">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>66</v>
+      </c>
+      <c r="B42">
+        <v>0</v>
+      </c>
+      <c r="C42">
+        <v>8</v>
+      </c>
+      <c r="D42">
+        <v>8</v>
+      </c>
+      <c r="E42">
+        <v>8</v>
+      </c>
+      <c r="F42">
+        <v>8</v>
+      </c>
+      <c r="G42">
+        <v>8</v>
+      </c>
+      <c r="H42">
+        <v>8</v>
+      </c>
+      <c r="I42">
+        <v>8</v>
+      </c>
+      <c r="J42">
+        <v>44</v>
+      </c>
+      <c r="K42">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>67</v>
+      </c>
+      <c r="B43">
+        <v>0</v>
+      </c>
+      <c r="C43">
+        <v>8</v>
+      </c>
+      <c r="D43">
+        <v>8</v>
+      </c>
+      <c r="E43">
+        <v>8</v>
+      </c>
+      <c r="F43">
+        <v>8</v>
+      </c>
+      <c r="G43">
+        <v>8</v>
+      </c>
+      <c r="H43">
+        <v>8</v>
+      </c>
+      <c r="I43">
+        <v>8</v>
+      </c>
+      <c r="J43">
+        <v>44</v>
+      </c>
+      <c r="K43">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>68</v>
+      </c>
+      <c r="B44">
+        <v>0</v>
+      </c>
+      <c r="C44">
+        <v>8</v>
+      </c>
+      <c r="D44">
+        <v>8</v>
+      </c>
+      <c r="E44">
+        <v>8</v>
+      </c>
+      <c r="F44">
+        <v>8</v>
+      </c>
+      <c r="G44">
+        <v>8</v>
+      </c>
+      <c r="H44">
+        <v>8</v>
+      </c>
+      <c r="I44">
+        <v>8</v>
+      </c>
+      <c r="J44">
+        <v>44</v>
+      </c>
+      <c r="K44">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>69</v>
+      </c>
+      <c r="B45">
+        <v>0</v>
+      </c>
+      <c r="C45">
+        <v>8</v>
+      </c>
+      <c r="D45">
+        <v>8</v>
+      </c>
+      <c r="E45">
+        <v>8</v>
+      </c>
+      <c r="F45">
+        <v>8</v>
+      </c>
+      <c r="G45">
+        <v>8</v>
+      </c>
+      <c r="H45">
+        <v>8</v>
+      </c>
+      <c r="I45">
+        <v>8</v>
+      </c>
+      <c r="J45">
+        <v>44</v>
+      </c>
+      <c r="K45">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>70</v>
+      </c>
+      <c r="B46">
+        <v>0</v>
+      </c>
+      <c r="C46">
+        <v>8</v>
+      </c>
+      <c r="D46">
+        <v>8</v>
+      </c>
+      <c r="E46">
+        <v>8</v>
+      </c>
+      <c r="F46">
+        <v>8</v>
+      </c>
+      <c r="G46">
+        <v>8</v>
+      </c>
+      <c r="H46">
+        <v>8</v>
+      </c>
+      <c r="I46">
+        <v>8</v>
+      </c>
+      <c r="J46">
+        <v>44</v>
+      </c>
+      <c r="K46">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>71</v>
+      </c>
+      <c r="B47">
+        <v>0</v>
+      </c>
+      <c r="C47">
+        <v>8</v>
+      </c>
+      <c r="D47">
+        <v>8</v>
+      </c>
+      <c r="E47">
+        <v>8</v>
+      </c>
+      <c r="F47">
+        <v>8</v>
+      </c>
+      <c r="G47">
+        <v>8</v>
+      </c>
+      <c r="H47">
+        <v>8</v>
+      </c>
+      <c r="I47">
+        <v>8</v>
+      </c>
+      <c r="J47">
+        <v>44</v>
+      </c>
+      <c r="K47">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>72</v>
+      </c>
+      <c r="B48">
+        <v>0</v>
+      </c>
+      <c r="C48">
+        <v>8</v>
+      </c>
+      <c r="D48">
+        <v>8</v>
+      </c>
+      <c r="E48">
+        <v>8</v>
+      </c>
+      <c r="F48">
+        <v>8</v>
+      </c>
+      <c r="G48">
+        <v>8</v>
+      </c>
+      <c r="H48">
+        <v>8</v>
+      </c>
+      <c r="I48">
+        <v>8</v>
+      </c>
+      <c r="J48">
+        <v>44</v>
+      </c>
+      <c r="K48">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>73</v>
+      </c>
+      <c r="B49">
+        <v>0</v>
+      </c>
+      <c r="C49">
+        <v>8</v>
+      </c>
+      <c r="D49">
+        <v>8</v>
+      </c>
+      <c r="E49">
+        <v>8</v>
+      </c>
+      <c r="F49">
+        <v>8</v>
+      </c>
+      <c r="G49">
+        <v>8</v>
+      </c>
+      <c r="H49">
+        <v>8</v>
+      </c>
+      <c r="I49">
+        <v>8</v>
+      </c>
+      <c r="J49">
+        <v>44</v>
+      </c>
+      <c r="K49">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>74</v>
+      </c>
+      <c r="B50">
+        <v>0</v>
+      </c>
+      <c r="C50">
+        <v>8</v>
+      </c>
+      <c r="D50">
+        <v>8</v>
+      </c>
+      <c r="E50">
+        <v>8</v>
+      </c>
+      <c r="F50">
+        <v>8</v>
+      </c>
+      <c r="G50">
+        <v>8</v>
+      </c>
+      <c r="H50">
+        <v>8</v>
+      </c>
+      <c r="I50">
+        <v>8</v>
+      </c>
+      <c r="J50">
+        <v>44</v>
+      </c>
+      <c r="K50">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>75</v>
+      </c>
+      <c r="B51">
+        <v>0</v>
+      </c>
+      <c r="C51">
+        <v>8</v>
+      </c>
+      <c r="D51">
+        <v>8</v>
+      </c>
+      <c r="E51">
+        <v>8</v>
+      </c>
+      <c r="F51">
+        <v>8</v>
+      </c>
+      <c r="G51">
+        <v>8</v>
+      </c>
+      <c r="H51">
+        <v>8</v>
+      </c>
+      <c r="I51">
+        <v>8</v>
+      </c>
+      <c r="J51">
+        <v>44</v>
+      </c>
+      <c r="K51">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>76</v>
+      </c>
+      <c r="B52">
+        <v>0</v>
+      </c>
+      <c r="C52">
+        <v>8</v>
+      </c>
+      <c r="D52">
+        <v>8</v>
+      </c>
+      <c r="E52">
+        <v>8</v>
+      </c>
+      <c r="F52">
+        <v>8</v>
+      </c>
+      <c r="G52">
+        <v>8</v>
+      </c>
+      <c r="H52">
+        <v>8</v>
+      </c>
+      <c r="I52">
+        <v>8</v>
+      </c>
+      <c r="J52">
+        <v>44</v>
+      </c>
+      <c r="K52">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>77</v>
+      </c>
+      <c r="B53">
+        <v>0</v>
+      </c>
+      <c r="C53">
+        <v>8</v>
+      </c>
+      <c r="D53">
+        <v>8</v>
+      </c>
+      <c r="E53">
+        <v>8</v>
+      </c>
+      <c r="F53">
+        <v>8</v>
+      </c>
+      <c r="G53">
+        <v>8</v>
+      </c>
+      <c r="H53">
+        <v>8</v>
+      </c>
+      <c r="I53">
+        <v>8</v>
+      </c>
+      <c r="J53">
+        <v>44</v>
+      </c>
+      <c r="K53">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>78</v>
+      </c>
+      <c r="B54">
+        <v>0</v>
+      </c>
+      <c r="C54">
+        <v>8</v>
+      </c>
+      <c r="D54">
+        <v>8</v>
+      </c>
+      <c r="E54">
+        <v>8</v>
+      </c>
+      <c r="F54">
+        <v>8</v>
+      </c>
+      <c r="G54">
+        <v>8</v>
+      </c>
+      <c r="H54">
+        <v>8</v>
+      </c>
+      <c r="I54">
+        <v>8</v>
+      </c>
+      <c r="J54">
+        <v>44</v>
+      </c>
+      <c r="K54">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>79</v>
+      </c>
+      <c r="B55">
+        <v>0</v>
+      </c>
+      <c r="C55">
+        <v>8</v>
+      </c>
+      <c r="D55">
+        <v>8</v>
+      </c>
+      <c r="E55">
+        <v>8</v>
+      </c>
+      <c r="F55">
+        <v>8</v>
+      </c>
+      <c r="G55">
+        <v>8</v>
+      </c>
+      <c r="H55">
+        <v>8</v>
+      </c>
+      <c r="I55">
+        <v>8</v>
+      </c>
+      <c r="J55">
+        <v>44</v>
+      </c>
+      <c r="K55">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>80</v>
+      </c>
+      <c r="B56">
+        <v>0</v>
+      </c>
+      <c r="C56">
+        <v>8</v>
+      </c>
+      <c r="D56">
+        <v>8</v>
+      </c>
+      <c r="E56">
+        <v>8</v>
+      </c>
+      <c r="F56">
+        <v>8</v>
+      </c>
+      <c r="G56">
+        <v>8</v>
+      </c>
+      <c r="H56">
+        <v>8</v>
+      </c>
+      <c r="I56">
+        <v>8</v>
+      </c>
+      <c r="J56">
+        <v>44</v>
+      </c>
+      <c r="K56">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>81</v>
+      </c>
+      <c r="B57">
+        <v>0</v>
+      </c>
+      <c r="C57">
+        <v>8</v>
+      </c>
+      <c r="D57">
+        <v>8</v>
+      </c>
+      <c r="E57">
+        <v>8</v>
+      </c>
+      <c r="F57">
+        <v>8</v>
+      </c>
+      <c r="G57">
+        <v>8</v>
+      </c>
+      <c r="H57">
+        <v>8</v>
+      </c>
+      <c r="I57">
+        <v>8</v>
+      </c>
+      <c r="J57">
+        <v>44</v>
+      </c>
+      <c r="K57">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>82</v>
+      </c>
+      <c r="B58">
+        <v>0</v>
+      </c>
+      <c r="C58">
+        <v>8</v>
+      </c>
+      <c r="D58">
+        <v>8</v>
+      </c>
+      <c r="E58">
+        <v>8</v>
+      </c>
+      <c r="F58">
+        <v>8</v>
+      </c>
+      <c r="G58">
+        <v>8</v>
+      </c>
+      <c r="H58">
+        <v>8</v>
+      </c>
+      <c r="I58">
+        <v>8</v>
+      </c>
+      <c r="J58">
+        <v>44</v>
+      </c>
+      <c r="K58">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>83</v>
+      </c>
+      <c r="B59">
+        <v>0</v>
+      </c>
+      <c r="C59">
+        <v>8</v>
+      </c>
+      <c r="D59">
+        <v>8</v>
+      </c>
+      <c r="E59">
+        <v>8</v>
+      </c>
+      <c r="F59">
+        <v>8</v>
+      </c>
+      <c r="G59">
+        <v>8</v>
+      </c>
+      <c r="H59">
+        <v>8</v>
+      </c>
+      <c r="I59">
+        <v>8</v>
+      </c>
+      <c r="J59">
+        <v>44</v>
+      </c>
+      <c r="K59">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>84</v>
+      </c>
+      <c r="B60">
+        <v>0</v>
+      </c>
+      <c r="C60">
+        <v>8</v>
+      </c>
+      <c r="D60">
+        <v>8</v>
+      </c>
+      <c r="E60">
+        <v>8</v>
+      </c>
+      <c r="F60">
+        <v>8</v>
+      </c>
+      <c r="G60">
+        <v>8</v>
+      </c>
+      <c r="H60">
+        <v>8</v>
+      </c>
+      <c r="I60">
+        <v>8</v>
+      </c>
+      <c r="J60">
+        <v>44</v>
+      </c>
+      <c r="K60">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>85</v>
+      </c>
+      <c r="B61">
+        <v>0</v>
+      </c>
+      <c r="C61">
+        <v>8</v>
+      </c>
+      <c r="D61">
+        <v>8</v>
+      </c>
+      <c r="E61">
+        <v>8</v>
+      </c>
+      <c r="F61">
+        <v>8</v>
+      </c>
+      <c r="G61">
+        <v>8</v>
+      </c>
+      <c r="H61">
+        <v>8</v>
+      </c>
+      <c r="I61">
+        <v>8</v>
+      </c>
+      <c r="J61">
+        <v>44</v>
+      </c>
+      <c r="K61">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>86</v>
+      </c>
+      <c r="B62">
+        <v>0</v>
+      </c>
+      <c r="C62">
+        <v>8</v>
+      </c>
+      <c r="D62">
+        <v>8</v>
+      </c>
+      <c r="E62">
+        <v>8</v>
+      </c>
+      <c r="F62">
+        <v>8</v>
+      </c>
+      <c r="G62">
+        <v>8</v>
+      </c>
+      <c r="H62">
+        <v>8</v>
+      </c>
+      <c r="I62">
+        <v>8</v>
+      </c>
+      <c r="J62">
+        <v>44</v>
+      </c>
+      <c r="K62">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>87</v>
+      </c>
+      <c r="B63">
+        <v>0</v>
+      </c>
+      <c r="C63">
+        <v>8</v>
+      </c>
+      <c r="D63">
+        <v>8</v>
+      </c>
+      <c r="E63">
+        <v>8</v>
+      </c>
+      <c r="F63">
+        <v>8</v>
+      </c>
+      <c r="G63">
+        <v>8</v>
+      </c>
+      <c r="H63">
+        <v>8</v>
+      </c>
+      <c r="I63">
+        <v>8</v>
+      </c>
+      <c r="J63">
+        <v>44</v>
+      </c>
+      <c r="K63">
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -832,554 +2913,655 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADABEAEA-84D9-4EB5-AA48-0815C68CC828}">
-  <dimension ref="A1:Y7"/>
+  <dimension ref="A1:Z8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+      <selection activeCell="B2" sqref="B2:Z8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.2" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="25" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="25" width="5.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B1" s="4">
-        <v>0.33333333333333331</v>
+        <v>0.375</v>
       </c>
       <c r="C1" s="4">
-        <v>0.35416666666666669</v>
+        <v>0.39583333333333298</v>
       </c>
       <c r="D1" s="4">
-        <v>0.375</v>
+        <v>0.41666666666666702</v>
       </c>
       <c r="E1" s="4">
-        <v>0.39583333333333298</v>
+        <v>0.4375</v>
       </c>
       <c r="F1" s="4">
-        <v>0.41666666666666702</v>
+        <v>0.45833333333333298</v>
       </c>
       <c r="G1" s="4">
-        <v>0.4375</v>
+        <v>0.47916666666666702</v>
       </c>
       <c r="H1" s="4">
-        <v>0.45833333333333298</v>
+        <v>0.5</v>
       </c>
       <c r="I1" s="4">
-        <v>0.47916666666666702</v>
+        <v>0.52083333333333304</v>
       </c>
       <c r="J1" s="4">
-        <v>0.5</v>
+        <v>0.54166666666666696</v>
       </c>
       <c r="K1" s="4">
-        <v>0.52083333333333304</v>
+        <v>0.5625</v>
       </c>
       <c r="L1" s="4">
-        <v>0.54166666666666696</v>
+        <v>0.58333333333333304</v>
       </c>
       <c r="M1" s="4">
-        <v>0.5625</v>
+        <v>0.60416666666666696</v>
       </c>
       <c r="N1" s="4">
-        <v>0.58333333333333304</v>
+        <v>0.625</v>
       </c>
       <c r="O1" s="4">
-        <v>0.60416666666666696</v>
+        <v>0.64583333333333404</v>
       </c>
       <c r="P1" s="4">
-        <v>0.625</v>
+        <v>0.66666666666666696</v>
       </c>
       <c r="Q1" s="4">
-        <v>0.64583333333333404</v>
+        <v>0.6875</v>
       </c>
       <c r="R1" s="4">
-        <v>0.66666666666666696</v>
+        <v>0.70833333333333404</v>
       </c>
       <c r="S1" s="4">
-        <v>0.6875</v>
+        <v>0.72916666666666696</v>
       </c>
       <c r="T1" s="4">
-        <v>0.70833333333333404</v>
+        <v>0.75</v>
       </c>
       <c r="U1" s="4">
-        <v>0.72916666666666696</v>
+        <v>0.77083333333333404</v>
       </c>
       <c r="V1" s="4">
-        <v>0.75</v>
+        <v>0.79166666666666696</v>
       </c>
       <c r="W1" s="4">
-        <v>0.77083333333333404</v>
+        <v>0.812500000000001</v>
       </c>
       <c r="X1" s="4">
-        <v>0.79166666666666696</v>
+        <v>0.83333333333333504</v>
       </c>
       <c r="Y1" s="4">
-        <v>0.812500000000001</v>
-      </c>
-    </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A2" s="8" t="s">
+        <v>0.85416666666666896</v>
+      </c>
+      <c r="Z1" s="4">
+        <v>0.875000000000003</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>6</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="C2">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="D2">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="E2">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="F2">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="G2">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="H2">
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="I2">
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="J2">
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="K2">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="L2">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="M2">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="N2">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="O2">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="P2">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="Q2">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="R2">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="S2">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="T2">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="U2">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="V2">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="W2">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="X2">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="Y2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A3" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="Z2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>7</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="E3">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="F3">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="G3">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="H3">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="I3">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="J3">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="K3">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="L3">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="M3">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="N3">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="O3">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="P3">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="Q3">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="R3">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="S3">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="T3">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="U3">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="V3">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="W3">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="X3">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="Y3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A4" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="Z3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>8</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="D4">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="E4">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="F4">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="G4">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="H4">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="I4">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="J4">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="K4">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="L4">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="M4">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="N4">
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="O4">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="P4">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="Q4">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="R4">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="S4">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="T4">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="U4">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="V4">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="W4">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="X4">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="Y4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A5" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="Z4">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>9</v>
       </c>
       <c r="B5">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="C5">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="D5">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="E5">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="F5">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="G5">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="H5">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="I5">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="J5">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="K5">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="L5">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="M5">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="N5">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="O5">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="P5">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="Q5">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="R5">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="S5">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="T5">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="U5">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="V5">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="W5">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="X5">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="Y5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A6" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="Z5">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>10</v>
       </c>
       <c r="B6">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="C6">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="D6">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="E6">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="F6">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="G6">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="H6">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="I6">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="J6">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="K6">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="L6">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="M6">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="N6">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="O6">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="P6">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="Q6">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="R6">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="S6">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="T6">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="U6">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="V6">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="W6">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="X6">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="Y6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A7" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="Z6">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>11</v>
       </c>
       <c r="B7">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="C7">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="D7">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="E7">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="F7">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="G7">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="H7">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="I7">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="J7">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="K7">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="L7">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="M7">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="N7">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="O7">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="P7">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="Q7">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="R7">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="S7">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="T7">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="U7">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="V7">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="W7">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="X7">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="Y7">
-        <v>2</v>
+        <v>15</v>
+      </c>
+      <c r="Z7">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8">
+        <v>15</v>
+      </c>
+      <c r="C8">
+        <v>15</v>
+      </c>
+      <c r="D8">
+        <v>15</v>
+      </c>
+      <c r="E8">
+        <v>15</v>
+      </c>
+      <c r="F8">
+        <v>15</v>
+      </c>
+      <c r="G8">
+        <v>15</v>
+      </c>
+      <c r="H8">
+        <v>25</v>
+      </c>
+      <c r="I8">
+        <v>25</v>
+      </c>
+      <c r="J8">
+        <v>25</v>
+      </c>
+      <c r="K8">
+        <v>25</v>
+      </c>
+      <c r="L8">
+        <v>25</v>
+      </c>
+      <c r="M8">
+        <v>25</v>
+      </c>
+      <c r="N8">
+        <v>25</v>
+      </c>
+      <c r="O8">
+        <v>25</v>
+      </c>
+      <c r="P8">
+        <v>25</v>
+      </c>
+      <c r="Q8">
+        <v>25</v>
+      </c>
+      <c r="R8">
+        <v>25</v>
+      </c>
+      <c r="S8">
+        <v>25</v>
+      </c>
+      <c r="T8">
+        <v>15</v>
+      </c>
+      <c r="U8">
+        <v>15</v>
+      </c>
+      <c r="V8">
+        <v>15</v>
+      </c>
+      <c r="W8">
+        <v>15</v>
+      </c>
+      <c r="X8">
+        <v>15</v>
+      </c>
+      <c r="Y8">
+        <v>15</v>
+      </c>
+      <c r="Z8">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -1389,15 +3571,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0550C504-3476-4905-9DF2-DC793A12066E}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.2" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>12</v>
       </c>
@@ -1405,53 +3587,82 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="8" t="s">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="6">
         <v>43934</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="8" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="6">
         <v>43935</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="8" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="6">
         <v>43936</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="8" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="6">
         <v>43937</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="8" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="6">
         <v>43938</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="8" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>11</v>
       </c>
       <c r="B7" s="6">
         <v>43939</v>
       </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" s="6">
+        <v>43940</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B9" s="6"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B10" s="6"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B11" s="6"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B12" s="6"/>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B13" s="6"/>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B14" s="6"/>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B15" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -1463,16 +3674,16 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.2" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="33" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.21875" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
@@ -1483,7 +3694,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -1494,18 +3705,18 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>21</v>
       </c>
       <c r="B3">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -1516,18 +3727,18 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>23</v>
       </c>
       <c r="B5">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -1535,28 +3746,37 @@
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="8" t="s">
-        <v>15</v>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7">
+        <v>56</v>
       </c>
       <c r="C7" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="8" t="s">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>14</v>
+      </c>
+      <c r="B8">
+        <v>44</v>
       </c>
       <c r="C8" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>25</v>
+      </c>
+      <c r="B9">
+        <v>10</v>
       </c>
       <c r="C9" t="s">
         <v>18</v>
@@ -1571,16 +3791,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF2FECBF-A4C3-4909-84B6-8E53240BA4DF}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.2" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.44140625" customWidth="1"/>
+    <col min="1" max="1" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>1</v>
       </c>
@@ -1588,12 +3808,15 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
Included constrainst on consecutive days working
</commit_message>
<xml_diff>
--- a/data/InputData.xlsx
+++ b/data/InputData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-20.04\home\renzo\PycharmProjects\workforce_scheduling\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39475F36-6460-4279-BCAF-FD47D73E0BC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D589ED85-19D9-4FB9-9751-7AA64FE1748C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="4" xr2:uid="{BCDF856C-6F0D-487F-8BC7-04FD1FA73F2E}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="89">
   <si>
     <t>Name</t>
   </si>
@@ -299,6 +299,9 @@
   </si>
   <si>
     <t>Leah</t>
+  </si>
+  <si>
+    <t>max_employee_consecutive_working_days</t>
   </si>
 </sst>
 </file>
@@ -3671,10 +3674,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{454F732D-22D4-429E-9B60-E7DB5EEF4D90}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3782,6 +3785,17 @@
         <v>18</v>
       </c>
     </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>88</v>
+      </c>
+      <c r="B10">
+        <v>6</v>
+      </c>
+      <c r="C10" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3792,7 +3806,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3812,9 +3826,6 @@
       <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2">
-        <v>120</v>
-      </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">

</xml_diff>

<commit_message>
Added constraint for working on sundays
</commit_message>
<xml_diff>
--- a/data/InputData.xlsx
+++ b/data/InputData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-20.04\home\renzo\PycharmProjects\workforce_scheduling\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E62AF565-6515-473F-A9CF-387B79698554}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BAA902F-5E06-4163-9632-7586661F999D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="3" xr2:uid="{BCDF856C-6F0D-487F-8BC7-04FD1FA73F2E}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{BCDF856C-6F0D-487F-8BC7-04FD1FA73F2E}"/>
   </bookViews>
   <sheets>
     <sheet name="Employees" sheetId="1" r:id="rId1"/>
@@ -718,8 +718,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56438F95-CB28-49F8-8745-B51411212C3C}">
   <dimension ref="A1:O63"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M1" sqref="M1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P23" sqref="P23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -802,7 +802,7 @@
         <v>8</v>
       </c>
       <c r="I2">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="J2">
         <v>56</v>
@@ -849,7 +849,7 @@
         <v>8</v>
       </c>
       <c r="I3">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="J3">
         <v>56</v>
@@ -896,7 +896,7 @@
         <v>8</v>
       </c>
       <c r="I4">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="J4">
         <v>56</v>
@@ -943,7 +943,7 @@
         <v>8</v>
       </c>
       <c r="I5">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="J5">
         <v>56</v>
@@ -990,7 +990,7 @@
         <v>8</v>
       </c>
       <c r="I6">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="J6">
         <v>56</v>
@@ -1037,7 +1037,7 @@
         <v>8</v>
       </c>
       <c r="I7">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="J7">
         <v>56</v>
@@ -1084,7 +1084,7 @@
         <v>8</v>
       </c>
       <c r="I8">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="J8">
         <v>56</v>
@@ -1131,7 +1131,7 @@
         <v>8</v>
       </c>
       <c r="I9">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="J9">
         <v>56</v>
@@ -1178,7 +1178,7 @@
         <v>8</v>
       </c>
       <c r="I10">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="J10">
         <v>56</v>
@@ -1225,7 +1225,7 @@
         <v>8</v>
       </c>
       <c r="I11">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="J11">
         <v>56</v>
@@ -1272,7 +1272,7 @@
         <v>8</v>
       </c>
       <c r="I12">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="J12">
         <v>56</v>
@@ -1319,7 +1319,7 @@
         <v>8</v>
       </c>
       <c r="I13">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="J13">
         <v>56</v>
@@ -1366,7 +1366,7 @@
         <v>8</v>
       </c>
       <c r="I14">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="J14">
         <v>56</v>
@@ -1413,7 +1413,7 @@
         <v>8</v>
       </c>
       <c r="I15">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="J15">
         <v>56</v>
@@ -1460,7 +1460,7 @@
         <v>8</v>
       </c>
       <c r="I16">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="J16">
         <v>56</v>
@@ -1507,7 +1507,7 @@
         <v>8</v>
       </c>
       <c r="I17">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="J17">
         <v>56</v>
@@ -1554,7 +1554,7 @@
         <v>8</v>
       </c>
       <c r="I18">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="J18">
         <v>56</v>
@@ -1601,7 +1601,7 @@
         <v>8</v>
       </c>
       <c r="I19">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="J19">
         <v>56</v>
@@ -1648,7 +1648,7 @@
         <v>8</v>
       </c>
       <c r="I20">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="J20">
         <v>56</v>
@@ -1695,7 +1695,7 @@
         <v>8</v>
       </c>
       <c r="I21">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="J21">
         <v>56</v>
@@ -1742,7 +1742,7 @@
         <v>8</v>
       </c>
       <c r="I22">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="J22">
         <v>56</v>
@@ -1789,7 +1789,7 @@
         <v>8</v>
       </c>
       <c r="I23">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="J23">
         <v>56</v>
@@ -1836,7 +1836,7 @@
         <v>8</v>
       </c>
       <c r="I24">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="J24">
         <v>56</v>
@@ -1883,7 +1883,7 @@
         <v>8</v>
       </c>
       <c r="I25">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="J25">
         <v>56</v>
@@ -1930,7 +1930,7 @@
         <v>8</v>
       </c>
       <c r="I26">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="J26">
         <v>56</v>
@@ -1977,7 +1977,7 @@
         <v>8</v>
       </c>
       <c r="I27">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="J27">
         <v>56</v>
@@ -2024,7 +2024,7 @@
         <v>8</v>
       </c>
       <c r="I28">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="J28">
         <v>56</v>
@@ -2071,7 +2071,7 @@
         <v>8</v>
       </c>
       <c r="I29">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="J29">
         <v>56</v>
@@ -2118,7 +2118,7 @@
         <v>8</v>
       </c>
       <c r="I30">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="J30">
         <v>56</v>
@@ -2127,7 +2127,7 @@
         <v>1</v>
       </c>
       <c r="L30">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M30">
         <v>2</v>
@@ -2165,7 +2165,7 @@
         <v>8</v>
       </c>
       <c r="I31">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="J31">
         <v>56</v>
@@ -2174,7 +2174,7 @@
         <v>3</v>
       </c>
       <c r="L31">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M31">
         <v>6</v>
@@ -2212,7 +2212,7 @@
         <v>8</v>
       </c>
       <c r="I32">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="J32">
         <v>56</v>
@@ -2221,7 +2221,7 @@
         <v>1</v>
       </c>
       <c r="L32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M32">
         <v>1</v>
@@ -2259,7 +2259,7 @@
         <v>8</v>
       </c>
       <c r="I33">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="J33">
         <v>56</v>
@@ -2268,7 +2268,7 @@
         <v>3</v>
       </c>
       <c r="L33">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M33">
         <v>1</v>
@@ -2306,7 +2306,7 @@
         <v>8</v>
       </c>
       <c r="I34">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="J34">
         <v>56</v>
@@ -2315,7 +2315,7 @@
         <v>1</v>
       </c>
       <c r="L34">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M34">
         <v>2</v>
@@ -2353,7 +2353,7 @@
         <v>8</v>
       </c>
       <c r="I35">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="J35">
         <v>56</v>
@@ -2362,7 +2362,7 @@
         <v>3</v>
       </c>
       <c r="L35">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M35">
         <v>0</v>
@@ -2400,7 +2400,7 @@
         <v>8</v>
       </c>
       <c r="I36">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="J36">
         <v>56</v>
@@ -2409,7 +2409,7 @@
         <v>1</v>
       </c>
       <c r="L36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M36">
         <v>1</v>
@@ -2447,7 +2447,7 @@
         <v>8</v>
       </c>
       <c r="I37">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="J37">
         <v>56</v>
@@ -2456,7 +2456,7 @@
         <v>3</v>
       </c>
       <c r="L37">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M37">
         <v>4</v>
@@ -2494,7 +2494,7 @@
         <v>8</v>
       </c>
       <c r="I38">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="J38">
         <v>56</v>
@@ -2503,7 +2503,7 @@
         <v>1</v>
       </c>
       <c r="L38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M38">
         <v>1</v>
@@ -2541,7 +2541,7 @@
         <v>8</v>
       </c>
       <c r="I39">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="J39">
         <v>56</v>
@@ -2550,7 +2550,7 @@
         <v>3</v>
       </c>
       <c r="L39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M39">
         <v>4</v>
@@ -2588,7 +2588,7 @@
         <v>8</v>
       </c>
       <c r="I40">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="J40">
         <v>56</v>
@@ -2597,7 +2597,7 @@
         <v>1</v>
       </c>
       <c r="L40">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M40">
         <v>4</v>
@@ -2635,7 +2635,7 @@
         <v>8</v>
       </c>
       <c r="I41">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="J41">
         <v>56</v>
@@ -2644,7 +2644,7 @@
         <v>3</v>
       </c>
       <c r="L41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M41">
         <v>1</v>
@@ -2682,7 +2682,7 @@
         <v>8</v>
       </c>
       <c r="I42">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="J42">
         <v>56</v>
@@ -2691,7 +2691,7 @@
         <v>1</v>
       </c>
       <c r="L42">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M42">
         <v>4</v>
@@ -2729,7 +2729,7 @@
         <v>8</v>
       </c>
       <c r="I43">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="J43">
         <v>56</v>
@@ -2738,7 +2738,7 @@
         <v>3</v>
       </c>
       <c r="L43">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M43">
         <v>1</v>
@@ -2776,7 +2776,7 @@
         <v>8</v>
       </c>
       <c r="I44">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="J44">
         <v>56</v>
@@ -2785,7 +2785,7 @@
         <v>1</v>
       </c>
       <c r="L44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M44">
         <v>0</v>
@@ -2823,7 +2823,7 @@
         <v>8</v>
       </c>
       <c r="I45">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="J45">
         <v>56</v>
@@ -2832,7 +2832,7 @@
         <v>3</v>
       </c>
       <c r="L45">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M45">
         <v>0</v>
@@ -2870,7 +2870,7 @@
         <v>8</v>
       </c>
       <c r="I46">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="J46">
         <v>56</v>
@@ -2879,7 +2879,7 @@
         <v>1</v>
       </c>
       <c r="L46">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M46">
         <v>0</v>
@@ -2917,7 +2917,7 @@
         <v>8</v>
       </c>
       <c r="I47">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="J47">
         <v>56</v>
@@ -2926,7 +2926,7 @@
         <v>3</v>
       </c>
       <c r="L47">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M47">
         <v>5</v>
@@ -2964,7 +2964,7 @@
         <v>8</v>
       </c>
       <c r="I48">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="J48">
         <v>56</v>
@@ -2973,7 +2973,7 @@
         <v>1</v>
       </c>
       <c r="L48">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M48">
         <v>1</v>
@@ -3011,7 +3011,7 @@
         <v>8</v>
       </c>
       <c r="I49">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="J49">
         <v>56</v>
@@ -3020,7 +3020,7 @@
         <v>3</v>
       </c>
       <c r="L49">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M49">
         <v>4</v>
@@ -3058,7 +3058,7 @@
         <v>8</v>
       </c>
       <c r="I50">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="J50">
         <v>56</v>
@@ -3067,7 +3067,7 @@
         <v>1</v>
       </c>
       <c r="L50">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M50">
         <v>3</v>
@@ -3105,7 +3105,7 @@
         <v>8</v>
       </c>
       <c r="I51">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="J51">
         <v>56</v>
@@ -3114,7 +3114,7 @@
         <v>3</v>
       </c>
       <c r="L51">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M51">
         <v>3</v>
@@ -3152,7 +3152,7 @@
         <v>8</v>
       </c>
       <c r="I52">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="J52">
         <v>56</v>
@@ -3161,7 +3161,7 @@
         <v>1</v>
       </c>
       <c r="L52">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M52">
         <v>1</v>
@@ -3199,7 +3199,7 @@
         <v>8</v>
       </c>
       <c r="I53">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="J53">
         <v>56</v>
@@ -3208,7 +3208,7 @@
         <v>3</v>
       </c>
       <c r="L53">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M53">
         <v>4</v>
@@ -3246,7 +3246,7 @@
         <v>8</v>
       </c>
       <c r="I54">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="J54">
         <v>56</v>
@@ -3255,7 +3255,7 @@
         <v>1</v>
       </c>
       <c r="L54">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M54">
         <v>4</v>
@@ -3293,7 +3293,7 @@
         <v>8</v>
       </c>
       <c r="I55">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="J55">
         <v>56</v>
@@ -3302,7 +3302,7 @@
         <v>3</v>
       </c>
       <c r="L55">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M55">
         <v>4</v>
@@ -3340,7 +3340,7 @@
         <v>8</v>
       </c>
       <c r="I56">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="J56">
         <v>56</v>
@@ -3349,7 +3349,7 @@
         <v>1</v>
       </c>
       <c r="L56">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M56">
         <v>1</v>
@@ -3387,7 +3387,7 @@
         <v>8</v>
       </c>
       <c r="I57">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="J57">
         <v>56</v>
@@ -3396,7 +3396,7 @@
         <v>3</v>
       </c>
       <c r="L57">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M57">
         <v>1</v>
@@ -3434,7 +3434,7 @@
         <v>8</v>
       </c>
       <c r="I58">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="J58">
         <v>56</v>
@@ -3443,7 +3443,7 @@
         <v>1</v>
       </c>
       <c r="L58">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M58">
         <v>4</v>
@@ -3481,7 +3481,7 @@
         <v>8</v>
       </c>
       <c r="I59">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="J59">
         <v>56</v>
@@ -3490,7 +3490,7 @@
         <v>3</v>
       </c>
       <c r="L59">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M59">
         <v>4</v>
@@ -3528,7 +3528,7 @@
         <v>8</v>
       </c>
       <c r="I60">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="J60">
         <v>56</v>
@@ -3537,7 +3537,7 @@
         <v>1</v>
       </c>
       <c r="L60">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M60">
         <v>5</v>
@@ -3575,7 +3575,7 @@
         <v>8</v>
       </c>
       <c r="I61">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="J61">
         <v>56</v>
@@ -3584,7 +3584,7 @@
         <v>3</v>
       </c>
       <c r="L61">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M61">
         <v>2</v>
@@ -3622,7 +3622,7 @@
         <v>8</v>
       </c>
       <c r="I62">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="J62">
         <v>56</v>
@@ -3631,7 +3631,7 @@
         <v>1</v>
       </c>
       <c r="L62">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M62">
         <v>1</v>
@@ -3669,7 +3669,7 @@
         <v>8</v>
       </c>
       <c r="I63">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="J63">
         <v>56</v>
@@ -3678,7 +3678,7 @@
         <v>3</v>
       </c>
       <c r="L63">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M63">
         <v>0</v>
@@ -4434,7 +4434,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{454F732D-22D4-429E-9B60-E7DB5EEF4D90}">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Included var for max employes in shift
</commit_message>
<xml_diff>
--- a/data/InputData.xlsx
+++ b/data/InputData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-20.04\home\renzo\PycharmProjects\workforce_scheduling\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2B492D0-B32E-46E5-9470-ED94F18408C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{646A995D-9A57-44B6-98AD-90485312EFBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="4" xr2:uid="{BCDF856C-6F0D-487F-8BC7-04FD1FA73F2E}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="103">
   <si>
     <t>Name</t>
   </si>
@@ -323,6 +323,9 @@
   </si>
   <si>
     <t>Max</t>
+  </si>
+  <si>
+    <t>max_extra_employees_per_shift</t>
   </si>
   <si>
     <t>regular_slots_per_day</t>
@@ -4080,7 +4083,7 @@
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B57">
         <v>8</v>
@@ -4127,7 +4130,7 @@
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B58">
         <v>8</v>
@@ -4174,7 +4177,7 @@
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B59">
         <v>8</v>
@@ -4221,7 +4224,7 @@
     </row>
     <row r="60" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B60">
         <v>8</v>
@@ -4268,7 +4271,7 @@
     </row>
     <row r="61" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B61">
         <v>8</v>
@@ -4315,7 +4318,7 @@
     </row>
     <row r="62" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B62">
         <v>8</v>
@@ -4362,7 +4365,7 @@
     </row>
     <row r="63" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B63">
         <v>8</v>
@@ -4515,10 +4518,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{454F732D-22D4-429E-9B60-E7DB5EEF4D90}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4672,7 +4675,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B14">
         <v>16</v>
@@ -4683,12 +4686,23 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B15">
         <v>4</v>
       </c>
       <c r="C15" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>93</v>
+      </c>
+      <c r="B16">
+        <v>2</v>
+      </c>
+      <c r="C16" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Incluida constraint de hora extra
</commit_message>
<xml_diff>
--- a/data/InputData.xlsx
+++ b/data/InputData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-20.04\home\renzo\PycharmProjects\workforce_scheduling\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{646A995D-9A57-44B6-98AD-90485312EFBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3E9F16C-BC52-43D3-911D-909996CC9228}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="4" xr2:uid="{BCDF856C-6F0D-487F-8BC7-04FD1FA73F2E}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="4" xr2:uid="{BCDF856C-6F0D-487F-8BC7-04FD1FA73F2E}"/>
   </bookViews>
   <sheets>
     <sheet name="Demand" sheetId="3" r:id="rId1"/>
@@ -1435,8 +1435,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56438F95-CB28-49F8-8745-B51411212C3C}">
   <dimension ref="A1:O63"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="A37" sqref="A1:XFD1048576"/>
+    <sheetView topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="J57" sqref="J57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1522,7 +1522,7 @@
         <v>8</v>
       </c>
       <c r="I2">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="J2">
         <v>56</v>
@@ -1569,7 +1569,7 @@
         <v>8</v>
       </c>
       <c r="I3">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="J3">
         <v>56</v>
@@ -1616,7 +1616,7 @@
         <v>8</v>
       </c>
       <c r="I4">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="J4">
         <v>56</v>
@@ -1663,7 +1663,7 @@
         <v>8</v>
       </c>
       <c r="I5">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="J5">
         <v>56</v>
@@ -1710,7 +1710,7 @@
         <v>8</v>
       </c>
       <c r="I6">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="J6">
         <v>56</v>
@@ -1757,7 +1757,7 @@
         <v>8</v>
       </c>
       <c r="I7">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="J7">
         <v>56</v>
@@ -1804,7 +1804,7 @@
         <v>8</v>
       </c>
       <c r="I8">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="J8">
         <v>56</v>
@@ -1851,7 +1851,7 @@
         <v>8</v>
       </c>
       <c r="I9">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="J9">
         <v>56</v>
@@ -1898,7 +1898,7 @@
         <v>8</v>
       </c>
       <c r="I10">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="J10">
         <v>56</v>
@@ -1945,7 +1945,7 @@
         <v>8</v>
       </c>
       <c r="I11">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="J11">
         <v>56</v>
@@ -1992,7 +1992,7 @@
         <v>8</v>
       </c>
       <c r="I12">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="J12">
         <v>56</v>
@@ -2039,7 +2039,7 @@
         <v>8</v>
       </c>
       <c r="I13">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="J13">
         <v>56</v>
@@ -2086,7 +2086,7 @@
         <v>8</v>
       </c>
       <c r="I14">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="J14">
         <v>56</v>
@@ -2133,7 +2133,7 @@
         <v>8</v>
       </c>
       <c r="I15">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="J15">
         <v>56</v>
@@ -2180,7 +2180,7 @@
         <v>8</v>
       </c>
       <c r="I16">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="J16">
         <v>56</v>
@@ -2227,7 +2227,7 @@
         <v>8</v>
       </c>
       <c r="I17">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="J17">
         <v>56</v>
@@ -2274,7 +2274,7 @@
         <v>8</v>
       </c>
       <c r="I18">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="J18">
         <v>56</v>
@@ -2321,7 +2321,7 @@
         <v>8</v>
       </c>
       <c r="I19">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="J19">
         <v>56</v>
@@ -2368,7 +2368,7 @@
         <v>8</v>
       </c>
       <c r="I20">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="J20">
         <v>56</v>
@@ -2415,7 +2415,7 @@
         <v>8</v>
       </c>
       <c r="I21">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="J21">
         <v>56</v>
@@ -2462,7 +2462,7 @@
         <v>8</v>
       </c>
       <c r="I22">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="J22">
         <v>56</v>
@@ -2509,7 +2509,7 @@
         <v>8</v>
       </c>
       <c r="I23">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="J23">
         <v>56</v>
@@ -2556,7 +2556,7 @@
         <v>8</v>
       </c>
       <c r="I24">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="J24">
         <v>56</v>
@@ -2603,7 +2603,7 @@
         <v>8</v>
       </c>
       <c r="I25">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="J25">
         <v>56</v>
@@ -2650,7 +2650,7 @@
         <v>8</v>
       </c>
       <c r="I26">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="J26">
         <v>56</v>
@@ -2697,7 +2697,7 @@
         <v>8</v>
       </c>
       <c r="I27">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="J27">
         <v>56</v>
@@ -2744,7 +2744,7 @@
         <v>8</v>
       </c>
       <c r="I28">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="J28">
         <v>56</v>
@@ -2791,7 +2791,7 @@
         <v>8</v>
       </c>
       <c r="I29">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="J29">
         <v>56</v>
@@ -2838,7 +2838,7 @@
         <v>8</v>
       </c>
       <c r="I30">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="J30">
         <v>56</v>
@@ -2885,7 +2885,7 @@
         <v>8</v>
       </c>
       <c r="I31">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="J31">
         <v>56</v>
@@ -2932,7 +2932,7 @@
         <v>8</v>
       </c>
       <c r="I32">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="J32">
         <v>56</v>
@@ -2979,7 +2979,7 @@
         <v>8</v>
       </c>
       <c r="I33">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="J33">
         <v>56</v>
@@ -3026,7 +3026,7 @@
         <v>8</v>
       </c>
       <c r="I34">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="J34">
         <v>56</v>
@@ -3073,7 +3073,7 @@
         <v>8</v>
       </c>
       <c r="I35">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="J35">
         <v>56</v>
@@ -3120,7 +3120,7 @@
         <v>8</v>
       </c>
       <c r="I36">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="J36">
         <v>56</v>
@@ -3167,7 +3167,7 @@
         <v>8</v>
       </c>
       <c r="I37">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="J37">
         <v>56</v>
@@ -3214,7 +3214,7 @@
         <v>8</v>
       </c>
       <c r="I38">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="J38">
         <v>56</v>
@@ -3261,7 +3261,7 @@
         <v>8</v>
       </c>
       <c r="I39">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="J39">
         <v>56</v>
@@ -3308,7 +3308,7 @@
         <v>8</v>
       </c>
       <c r="I40">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="J40">
         <v>56</v>
@@ -3355,7 +3355,7 @@
         <v>8</v>
       </c>
       <c r="I41">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="J41">
         <v>56</v>
@@ -3402,7 +3402,7 @@
         <v>8</v>
       </c>
       <c r="I42">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="J42">
         <v>56</v>
@@ -3449,7 +3449,7 @@
         <v>8</v>
       </c>
       <c r="I43">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="J43">
         <v>56</v>
@@ -3496,7 +3496,7 @@
         <v>8</v>
       </c>
       <c r="I44">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="J44">
         <v>56</v>
@@ -3543,7 +3543,7 @@
         <v>8</v>
       </c>
       <c r="I45">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="J45">
         <v>56</v>
@@ -3590,7 +3590,7 @@
         <v>8</v>
       </c>
       <c r="I46">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="J46">
         <v>56</v>
@@ -3637,7 +3637,7 @@
         <v>8</v>
       </c>
       <c r="I47">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="J47">
         <v>56</v>
@@ -3684,7 +3684,7 @@
         <v>8</v>
       </c>
       <c r="I48">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="J48">
         <v>56</v>
@@ -3731,7 +3731,7 @@
         <v>8</v>
       </c>
       <c r="I49">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="J49">
         <v>56</v>
@@ -3778,7 +3778,7 @@
         <v>8</v>
       </c>
       <c r="I50">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="J50">
         <v>56</v>
@@ -3825,7 +3825,7 @@
         <v>8</v>
       </c>
       <c r="I51">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="J51">
         <v>56</v>
@@ -3872,7 +3872,7 @@
         <v>8</v>
       </c>
       <c r="I52">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="J52">
         <v>56</v>
@@ -3919,7 +3919,7 @@
         <v>8</v>
       </c>
       <c r="I53">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="J53">
         <v>56</v>
@@ -3966,7 +3966,7 @@
         <v>8</v>
       </c>
       <c r="I54">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="J54">
         <v>56</v>
@@ -4013,7 +4013,7 @@
         <v>8</v>
       </c>
       <c r="I55">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="J55">
         <v>56</v>
@@ -4060,7 +4060,7 @@
         <v>8</v>
       </c>
       <c r="I56">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="J56">
         <v>56</v>
@@ -4107,7 +4107,7 @@
         <v>8</v>
       </c>
       <c r="I57">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="J57">
         <v>56</v>
@@ -4154,7 +4154,7 @@
         <v>8</v>
       </c>
       <c r="I58">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="J58">
         <v>56</v>
@@ -4201,7 +4201,7 @@
         <v>8</v>
       </c>
       <c r="I59">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="J59">
         <v>56</v>
@@ -4248,7 +4248,7 @@
         <v>8</v>
       </c>
       <c r="I60">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="J60">
         <v>56</v>
@@ -4295,7 +4295,7 @@
         <v>8</v>
       </c>
       <c r="I61">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="J61">
         <v>56</v>
@@ -4342,7 +4342,7 @@
         <v>8</v>
       </c>
       <c r="I62">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="J62">
         <v>56</v>
@@ -4389,7 +4389,7 @@
         <v>8</v>
       </c>
       <c r="I63">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="J63">
         <v>56</v>
@@ -4521,7 +4521,7 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Working solutions with min of 30 hour per day
</commit_message>
<xml_diff>
--- a/data/InputData.xlsx
+++ b/data/InputData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-20.04\home\renzo\PycharmProjects\workforce_scheduling\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3E9F16C-BC52-43D3-911D-909996CC9228}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1697F5D0-61EE-46D2-A2D7-9EE42EA973CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="4" xr2:uid="{BCDF856C-6F0D-487F-8BC7-04FD1FA73F2E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{BCDF856C-6F0D-487F-8BC7-04FD1FA73F2E}"/>
   </bookViews>
   <sheets>
     <sheet name="Demand" sheetId="3" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="101">
   <si>
     <t>Name</t>
   </si>
@@ -347,12 +347,6 @@
   </si>
   <si>
     <t>Nicole</t>
-  </si>
-  <si>
-    <t>Jacob</t>
-  </si>
-  <si>
-    <t>Leah</t>
   </si>
 </sst>
 </file>
@@ -1433,10 +1427,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56438F95-CB28-49F8-8745-B51411212C3C}">
-  <dimension ref="A1:O63"/>
+  <dimension ref="A1:O61"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="J57" sqref="J57"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="A62" sqref="A62:XFD63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1522,7 +1516,7 @@
         <v>8</v>
       </c>
       <c r="I2">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="J2">
         <v>56</v>
@@ -1569,7 +1563,7 @@
         <v>8</v>
       </c>
       <c r="I3">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="J3">
         <v>56</v>
@@ -1616,7 +1610,7 @@
         <v>8</v>
       </c>
       <c r="I4">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="J4">
         <v>56</v>
@@ -1663,7 +1657,7 @@
         <v>8</v>
       </c>
       <c r="I5">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="J5">
         <v>56</v>
@@ -1710,7 +1704,7 @@
         <v>8</v>
       </c>
       <c r="I6">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="J6">
         <v>56</v>
@@ -1757,7 +1751,7 @@
         <v>8</v>
       </c>
       <c r="I7">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="J7">
         <v>56</v>
@@ -1804,7 +1798,7 @@
         <v>8</v>
       </c>
       <c r="I8">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="J8">
         <v>56</v>
@@ -1851,7 +1845,7 @@
         <v>8</v>
       </c>
       <c r="I9">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="J9">
         <v>56</v>
@@ -1898,7 +1892,7 @@
         <v>8</v>
       </c>
       <c r="I10">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="J10">
         <v>56</v>
@@ -1945,7 +1939,7 @@
         <v>8</v>
       </c>
       <c r="I11">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="J11">
         <v>56</v>
@@ -1992,7 +1986,7 @@
         <v>8</v>
       </c>
       <c r="I12">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="J12">
         <v>56</v>
@@ -2039,7 +2033,7 @@
         <v>8</v>
       </c>
       <c r="I13">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="J13">
         <v>56</v>
@@ -2086,7 +2080,7 @@
         <v>8</v>
       </c>
       <c r="I14">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="J14">
         <v>56</v>
@@ -2133,7 +2127,7 @@
         <v>8</v>
       </c>
       <c r="I15">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="J15">
         <v>56</v>
@@ -2180,7 +2174,7 @@
         <v>8</v>
       </c>
       <c r="I16">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="J16">
         <v>56</v>
@@ -2227,7 +2221,7 @@
         <v>8</v>
       </c>
       <c r="I17">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="J17">
         <v>56</v>
@@ -2274,7 +2268,7 @@
         <v>8</v>
       </c>
       <c r="I18">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="J18">
         <v>56</v>
@@ -2321,7 +2315,7 @@
         <v>8</v>
       </c>
       <c r="I19">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="J19">
         <v>56</v>
@@ -2368,7 +2362,7 @@
         <v>8</v>
       </c>
       <c r="I20">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="J20">
         <v>56</v>
@@ -2415,7 +2409,7 @@
         <v>8</v>
       </c>
       <c r="I21">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="J21">
         <v>56</v>
@@ -2462,7 +2456,7 @@
         <v>8</v>
       </c>
       <c r="I22">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="J22">
         <v>56</v>
@@ -2509,7 +2503,7 @@
         <v>8</v>
       </c>
       <c r="I23">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="J23">
         <v>56</v>
@@ -2556,7 +2550,7 @@
         <v>8</v>
       </c>
       <c r="I24">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="J24">
         <v>56</v>
@@ -2603,7 +2597,7 @@
         <v>8</v>
       </c>
       <c r="I25">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="J25">
         <v>56</v>
@@ -2650,7 +2644,7 @@
         <v>8</v>
       </c>
       <c r="I26">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="J26">
         <v>56</v>
@@ -2697,7 +2691,7 @@
         <v>8</v>
       </c>
       <c r="I27">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="J27">
         <v>56</v>
@@ -2744,7 +2738,7 @@
         <v>8</v>
       </c>
       <c r="I28">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="J28">
         <v>56</v>
@@ -2791,7 +2785,7 @@
         <v>8</v>
       </c>
       <c r="I29">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="J29">
         <v>56</v>
@@ -2838,7 +2832,7 @@
         <v>8</v>
       </c>
       <c r="I30">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="J30">
         <v>56</v>
@@ -2885,7 +2879,7 @@
         <v>8</v>
       </c>
       <c r="I31">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="J31">
         <v>56</v>
@@ -2932,7 +2926,7 @@
         <v>8</v>
       </c>
       <c r="I32">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="J32">
         <v>56</v>
@@ -2979,7 +2973,7 @@
         <v>8</v>
       </c>
       <c r="I33">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="J33">
         <v>56</v>
@@ -3026,7 +3020,7 @@
         <v>8</v>
       </c>
       <c r="I34">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="J34">
         <v>56</v>
@@ -3073,7 +3067,7 @@
         <v>8</v>
       </c>
       <c r="I35">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="J35">
         <v>56</v>
@@ -3120,7 +3114,7 @@
         <v>8</v>
       </c>
       <c r="I36">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="J36">
         <v>56</v>
@@ -3167,7 +3161,7 @@
         <v>8</v>
       </c>
       <c r="I37">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="J37">
         <v>56</v>
@@ -3214,7 +3208,7 @@
         <v>8</v>
       </c>
       <c r="I38">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="J38">
         <v>56</v>
@@ -3261,7 +3255,7 @@
         <v>8</v>
       </c>
       <c r="I39">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="J39">
         <v>56</v>
@@ -3308,7 +3302,7 @@
         <v>8</v>
       </c>
       <c r="I40">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="J40">
         <v>56</v>
@@ -3355,7 +3349,7 @@
         <v>8</v>
       </c>
       <c r="I41">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="J41">
         <v>56</v>
@@ -3402,7 +3396,7 @@
         <v>8</v>
       </c>
       <c r="I42">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="J42">
         <v>56</v>
@@ -3449,7 +3443,7 @@
         <v>8</v>
       </c>
       <c r="I43">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="J43">
         <v>56</v>
@@ -3496,7 +3490,7 @@
         <v>8</v>
       </c>
       <c r="I44">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="J44">
         <v>56</v>
@@ -3543,7 +3537,7 @@
         <v>8</v>
       </c>
       <c r="I45">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="J45">
         <v>56</v>
@@ -3590,7 +3584,7 @@
         <v>8</v>
       </c>
       <c r="I46">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="J46">
         <v>56</v>
@@ -3637,7 +3631,7 @@
         <v>8</v>
       </c>
       <c r="I47">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="J47">
         <v>56</v>
@@ -3684,7 +3678,7 @@
         <v>8</v>
       </c>
       <c r="I48">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="J48">
         <v>56</v>
@@ -3731,7 +3725,7 @@
         <v>8</v>
       </c>
       <c r="I49">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="J49">
         <v>56</v>
@@ -3778,7 +3772,7 @@
         <v>8</v>
       </c>
       <c r="I50">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="J50">
         <v>56</v>
@@ -3825,7 +3819,7 @@
         <v>8</v>
       </c>
       <c r="I51">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="J51">
         <v>56</v>
@@ -3872,7 +3866,7 @@
         <v>8</v>
       </c>
       <c r="I52">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="J52">
         <v>56</v>
@@ -3919,7 +3913,7 @@
         <v>8</v>
       </c>
       <c r="I53">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="J53">
         <v>56</v>
@@ -3966,7 +3960,7 @@
         <v>8</v>
       </c>
       <c r="I54">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="J54">
         <v>56</v>
@@ -4013,7 +4007,7 @@
         <v>8</v>
       </c>
       <c r="I55">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="J55">
         <v>56</v>
@@ -4060,7 +4054,7 @@
         <v>8</v>
       </c>
       <c r="I56">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="J56">
         <v>56</v>
@@ -4107,7 +4101,7 @@
         <v>8</v>
       </c>
       <c r="I57">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="J57">
         <v>56</v>
@@ -4154,7 +4148,7 @@
         <v>8</v>
       </c>
       <c r="I58">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="J58">
         <v>56</v>
@@ -4201,7 +4195,7 @@
         <v>8</v>
       </c>
       <c r="I59">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="J59">
         <v>56</v>
@@ -4248,7 +4242,7 @@
         <v>8</v>
       </c>
       <c r="I60">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="J60">
         <v>56</v>
@@ -4295,7 +4289,7 @@
         <v>8</v>
       </c>
       <c r="I61">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="J61">
         <v>56</v>
@@ -4313,100 +4307,6 @@
         <v>0</v>
       </c>
       <c r="O61">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>101</v>
-      </c>
-      <c r="B62">
-        <v>8</v>
-      </c>
-      <c r="C62">
-        <v>8</v>
-      </c>
-      <c r="D62">
-        <v>8</v>
-      </c>
-      <c r="E62">
-        <v>8</v>
-      </c>
-      <c r="F62">
-        <v>8</v>
-      </c>
-      <c r="G62">
-        <v>8</v>
-      </c>
-      <c r="H62">
-        <v>8</v>
-      </c>
-      <c r="I62">
-        <v>0</v>
-      </c>
-      <c r="J62">
-        <v>56</v>
-      </c>
-      <c r="K62">
-        <v>1</v>
-      </c>
-      <c r="L62">
-        <v>0</v>
-      </c>
-      <c r="M62">
-        <v>1</v>
-      </c>
-      <c r="N62">
-        <v>0</v>
-      </c>
-      <c r="O62">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>102</v>
-      </c>
-      <c r="B63">
-        <v>8</v>
-      </c>
-      <c r="C63">
-        <v>8</v>
-      </c>
-      <c r="D63">
-        <v>8</v>
-      </c>
-      <c r="E63">
-        <v>8</v>
-      </c>
-      <c r="F63">
-        <v>8</v>
-      </c>
-      <c r="G63">
-        <v>8</v>
-      </c>
-      <c r="H63">
-        <v>8</v>
-      </c>
-      <c r="I63">
-        <v>0</v>
-      </c>
-      <c r="J63">
-        <v>56</v>
-      </c>
-      <c r="K63">
-        <v>3</v>
-      </c>
-      <c r="L63">
-        <v>0</v>
-      </c>
-      <c r="M63">
-        <v>0</v>
-      </c>
-      <c r="N63">
-        <v>0</v>
-      </c>
-      <c r="O63">
         <v>0</v>
       </c>
     </row>
@@ -4520,8 +4420,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{454F732D-22D4-429E-9B60-E7DB5EEF4D90}">
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4568,7 +4468,7 @@
         <v>21</v>
       </c>
       <c r="B4">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C4" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
Adicionadas instruções para rodar projeto
</commit_message>
<xml_diff>
--- a/data/InputData.xlsx
+++ b/data/InputData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-20.04\home\renzo\PycharmProjects\workforce_scheduling\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1697F5D0-61EE-46D2-A2D7-9EE42EA973CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51A3B021-450F-4547-B6A7-2A6BD88839DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{BCDF856C-6F0D-487F-8BC7-04FD1FA73F2E}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="98">
   <si>
     <t>Name</t>
   </si>
@@ -338,15 +338,6 @@
   </si>
   <si>
     <t>Philip</t>
-  </si>
-  <si>
-    <t>Tina</t>
-  </si>
-  <si>
-    <t>Simon</t>
-  </si>
-  <si>
-    <t>Nicole</t>
   </si>
 </sst>
 </file>
@@ -1427,10 +1418,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56438F95-CB28-49F8-8745-B51411212C3C}">
-  <dimension ref="A1:O61"/>
+  <dimension ref="A1:O58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="A62" sqref="A62:XFD63"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="J54" sqref="J54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1516,7 +1507,7 @@
         <v>8</v>
       </c>
       <c r="I2">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="J2">
         <v>56</v>
@@ -1563,7 +1554,7 @@
         <v>8</v>
       </c>
       <c r="I3">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="J3">
         <v>56</v>
@@ -1610,7 +1601,7 @@
         <v>8</v>
       </c>
       <c r="I4">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="J4">
         <v>56</v>
@@ -1657,7 +1648,7 @@
         <v>8</v>
       </c>
       <c r="I5">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="J5">
         <v>56</v>
@@ -1704,7 +1695,7 @@
         <v>8</v>
       </c>
       <c r="I6">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="J6">
         <v>56</v>
@@ -1751,7 +1742,7 @@
         <v>8</v>
       </c>
       <c r="I7">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="J7">
         <v>56</v>
@@ -1798,7 +1789,7 @@
         <v>8</v>
       </c>
       <c r="I8">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="J8">
         <v>56</v>
@@ -1845,7 +1836,7 @@
         <v>8</v>
       </c>
       <c r="I9">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="J9">
         <v>56</v>
@@ -1892,7 +1883,7 @@
         <v>8</v>
       </c>
       <c r="I10">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="J10">
         <v>56</v>
@@ -1939,7 +1930,7 @@
         <v>8</v>
       </c>
       <c r="I11">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="J11">
         <v>56</v>
@@ -1986,7 +1977,7 @@
         <v>8</v>
       </c>
       <c r="I12">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="J12">
         <v>56</v>
@@ -2033,7 +2024,7 @@
         <v>8</v>
       </c>
       <c r="I13">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="J13">
         <v>56</v>
@@ -2080,7 +2071,7 @@
         <v>8</v>
       </c>
       <c r="I14">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="J14">
         <v>56</v>
@@ -2127,7 +2118,7 @@
         <v>8</v>
       </c>
       <c r="I15">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="J15">
         <v>56</v>
@@ -2174,7 +2165,7 @@
         <v>8</v>
       </c>
       <c r="I16">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="J16">
         <v>56</v>
@@ -2221,7 +2212,7 @@
         <v>8</v>
       </c>
       <c r="I17">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="J17">
         <v>56</v>
@@ -2268,7 +2259,7 @@
         <v>8</v>
       </c>
       <c r="I18">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="J18">
         <v>56</v>
@@ -2315,7 +2306,7 @@
         <v>8</v>
       </c>
       <c r="I19">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="J19">
         <v>56</v>
@@ -2362,7 +2353,7 @@
         <v>8</v>
       </c>
       <c r="I20">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="J20">
         <v>56</v>
@@ -2409,7 +2400,7 @@
         <v>8</v>
       </c>
       <c r="I21">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="J21">
         <v>56</v>
@@ -2456,7 +2447,7 @@
         <v>8</v>
       </c>
       <c r="I22">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="J22">
         <v>56</v>
@@ -2503,7 +2494,7 @@
         <v>8</v>
       </c>
       <c r="I23">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="J23">
         <v>56</v>
@@ -2550,7 +2541,7 @@
         <v>8</v>
       </c>
       <c r="I24">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="J24">
         <v>56</v>
@@ -2597,7 +2588,7 @@
         <v>8</v>
       </c>
       <c r="I25">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="J25">
         <v>56</v>
@@ -2644,7 +2635,7 @@
         <v>8</v>
       </c>
       <c r="I26">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="J26">
         <v>56</v>
@@ -2691,7 +2682,7 @@
         <v>8</v>
       </c>
       <c r="I27">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="J27">
         <v>56</v>
@@ -2738,7 +2729,7 @@
         <v>8</v>
       </c>
       <c r="I28">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="J28">
         <v>56</v>
@@ -2785,7 +2776,7 @@
         <v>8</v>
       </c>
       <c r="I29">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="J29">
         <v>56</v>
@@ -2832,7 +2823,7 @@
         <v>8</v>
       </c>
       <c r="I30">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="J30">
         <v>56</v>
@@ -2879,7 +2870,7 @@
         <v>8</v>
       </c>
       <c r="I31">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="J31">
         <v>56</v>
@@ -2926,7 +2917,7 @@
         <v>8</v>
       </c>
       <c r="I32">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="J32">
         <v>56</v>
@@ -2973,7 +2964,7 @@
         <v>8</v>
       </c>
       <c r="I33">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="J33">
         <v>56</v>
@@ -3020,7 +3011,7 @@
         <v>8</v>
       </c>
       <c r="I34">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="J34">
         <v>56</v>
@@ -3067,7 +3058,7 @@
         <v>8</v>
       </c>
       <c r="I35">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="J35">
         <v>56</v>
@@ -3114,7 +3105,7 @@
         <v>8</v>
       </c>
       <c r="I36">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="J36">
         <v>56</v>
@@ -3161,7 +3152,7 @@
         <v>8</v>
       </c>
       <c r="I37">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="J37">
         <v>56</v>
@@ -3208,7 +3199,7 @@
         <v>8</v>
       </c>
       <c r="I38">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="J38">
         <v>56</v>
@@ -3255,7 +3246,7 @@
         <v>8</v>
       </c>
       <c r="I39">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="J39">
         <v>56</v>
@@ -3302,7 +3293,7 @@
         <v>8</v>
       </c>
       <c r="I40">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="J40">
         <v>56</v>
@@ -3349,7 +3340,7 @@
         <v>8</v>
       </c>
       <c r="I41">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="J41">
         <v>56</v>
@@ -3396,7 +3387,7 @@
         <v>8</v>
       </c>
       <c r="I42">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="J42">
         <v>56</v>
@@ -3443,7 +3434,7 @@
         <v>8</v>
       </c>
       <c r="I43">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="J43">
         <v>56</v>
@@ -3490,7 +3481,7 @@
         <v>8</v>
       </c>
       <c r="I44">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="J44">
         <v>56</v>
@@ -3537,7 +3528,7 @@
         <v>8</v>
       </c>
       <c r="I45">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="J45">
         <v>56</v>
@@ -3584,7 +3575,7 @@
         <v>8</v>
       </c>
       <c r="I46">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="J46">
         <v>56</v>
@@ -3631,7 +3622,7 @@
         <v>8</v>
       </c>
       <c r="I47">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="J47">
         <v>56</v>
@@ -3678,7 +3669,7 @@
         <v>8</v>
       </c>
       <c r="I48">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="J48">
         <v>56</v>
@@ -3725,7 +3716,7 @@
         <v>8</v>
       </c>
       <c r="I49">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="J49">
         <v>56</v>
@@ -3772,7 +3763,7 @@
         <v>8</v>
       </c>
       <c r="I50">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="J50">
         <v>56</v>
@@ -3819,7 +3810,7 @@
         <v>8</v>
       </c>
       <c r="I51">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="J51">
         <v>56</v>
@@ -3866,7 +3857,7 @@
         <v>8</v>
       </c>
       <c r="I52">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="J52">
         <v>56</v>
@@ -3913,7 +3904,7 @@
         <v>8</v>
       </c>
       <c r="I53">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="J53">
         <v>56</v>
@@ -3960,7 +3951,7 @@
         <v>8</v>
       </c>
       <c r="I54">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="J54">
         <v>56</v>
@@ -4007,7 +3998,7 @@
         <v>8</v>
       </c>
       <c r="I55">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="J55">
         <v>56</v>
@@ -4054,7 +4045,7 @@
         <v>8</v>
       </c>
       <c r="I56">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="J56">
         <v>56</v>
@@ -4101,7 +4092,7 @@
         <v>8</v>
       </c>
       <c r="I57">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="J57">
         <v>56</v>
@@ -4148,7 +4139,7 @@
         <v>8</v>
       </c>
       <c r="I58">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="J58">
         <v>56</v>
@@ -4166,147 +4157,6 @@
         <v>0</v>
       </c>
       <c r="O58">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>98</v>
-      </c>
-      <c r="B59">
-        <v>8</v>
-      </c>
-      <c r="C59">
-        <v>8</v>
-      </c>
-      <c r="D59">
-        <v>8</v>
-      </c>
-      <c r="E59">
-        <v>8</v>
-      </c>
-      <c r="F59">
-        <v>8</v>
-      </c>
-      <c r="G59">
-        <v>8</v>
-      </c>
-      <c r="H59">
-        <v>8</v>
-      </c>
-      <c r="I59">
-        <v>30</v>
-      </c>
-      <c r="J59">
-        <v>56</v>
-      </c>
-      <c r="K59">
-        <v>3</v>
-      </c>
-      <c r="L59">
-        <v>0</v>
-      </c>
-      <c r="M59">
-        <v>4</v>
-      </c>
-      <c r="N59">
-        <v>0</v>
-      </c>
-      <c r="O59">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>99</v>
-      </c>
-      <c r="B60">
-        <v>8</v>
-      </c>
-      <c r="C60">
-        <v>8</v>
-      </c>
-      <c r="D60">
-        <v>8</v>
-      </c>
-      <c r="E60">
-        <v>8</v>
-      </c>
-      <c r="F60">
-        <v>8</v>
-      </c>
-      <c r="G60">
-        <v>8</v>
-      </c>
-      <c r="H60">
-        <v>8</v>
-      </c>
-      <c r="I60">
-        <v>30</v>
-      </c>
-      <c r="J60">
-        <v>56</v>
-      </c>
-      <c r="K60">
-        <v>1</v>
-      </c>
-      <c r="L60">
-        <v>0</v>
-      </c>
-      <c r="M60">
-        <v>5</v>
-      </c>
-      <c r="N60">
-        <v>0</v>
-      </c>
-      <c r="O60">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>100</v>
-      </c>
-      <c r="B61">
-        <v>8</v>
-      </c>
-      <c r="C61">
-        <v>8</v>
-      </c>
-      <c r="D61">
-        <v>8</v>
-      </c>
-      <c r="E61">
-        <v>8</v>
-      </c>
-      <c r="F61">
-        <v>8</v>
-      </c>
-      <c r="G61">
-        <v>8</v>
-      </c>
-      <c r="H61">
-        <v>8</v>
-      </c>
-      <c r="I61">
-        <v>30</v>
-      </c>
-      <c r="J61">
-        <v>56</v>
-      </c>
-      <c r="K61">
-        <v>3</v>
-      </c>
-      <c r="L61">
-        <v>0</v>
-      </c>
-      <c r="M61">
-        <v>2</v>
-      </c>
-      <c r="N61">
-        <v>0</v>
-      </c>
-      <c r="O61">
         <v>0</v>
       </c>
     </row>

</xml_diff>